<commit_message>
Adding SQL file - 12/12/21
</commit_message>
<xml_diff>
--- a/Simple Height Weight/sample.xlsx
+++ b/Simple Height Weight/sample.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4ff194ff2a14eaee/Desktop/Obinna-Jason-NwokeII-DataSciencePortfolio/Simple Height Weight/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="11_F25DC773A252ABDACC1048B2291D487A5ADE58E9" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{81339EBD-7BE5-45CF-BD8C-61E35610EB85}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="11_F25DC773A252ABDACC1048B2291D487A5ADE58E9" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E0D16AD8-D243-4541-9CCF-D8C45BC51C7E}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2573,5 +2573,8 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <customProperties>
+    <customPr name="LastActive" r:id="rId2"/>
+  </customProperties>
 </worksheet>
 </file>
</xml_diff>